<commit_message>
Corrected error in convergence table
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
@@ -104,6 +104,21 @@
     <t>Green</t>
   </si>
   <si>
+    <t>[0.17381931436989675, 0.015704630897802694, 0.0050889346986909955, 0.0008049994197372305, 0.00020964279836201426]</t>
+  </si>
+  <si>
+    <t>squareWithDelaunayTriangles</t>
+  </si>
+  <si>
+    <t>[u'squareWithTriangles_1', u'squareWithTriangles_2', u'squareWithTriangles_3', u'squareWithTriangles_4', u'squareWithTriangles_5']</t>
+  </si>
+  <si>
+    <t>[6.32455532033676, 14.966629547095765, 30.561413579872255, 80.13738203859668, 160.8477541030648]</t>
+  </si>
+  <si>
+    <t>Unstructured_triangles</t>
+  </si>
+  <si>
     <t>[0.033558391102700875, 0.008265416966230732, 0.0020587067645389525, 0.0009143535530498623]</t>
   </si>
   <si>
@@ -137,27 +152,12 @@
     <t>Unstructured_Tetrahedra</t>
   </si>
   <si>
-    <t>[0.17381931436989675, 0.015704630897802694, 0.0050889346986909955, 0.0008049994197372305, 0.00020964279836201426]</t>
+    <t>[0.0335583911027002, 0.0020587067645353673, 0.0003290517629436336, 8.22507622070037e-05, 2.0561929520719267e-05, 5.140434811781161e-06]</t>
   </si>
   <si>
     <t>Squares</t>
   </si>
   <si>
-    <t>squareWithDelaunayTriangles</t>
-  </si>
-  <si>
-    <t>[u'squareWithTriangles_1', u'squareWithTriangles_2', u'squareWithTriangles_3', u'squareWithTriangles_4', u'squareWithTriangles_5']</t>
-  </si>
-  <si>
-    <t>[6.32455532033676, 14.966629547095765, 30.561413579872255, 80.13738203859668, 160.8477541030648]</t>
-  </si>
-  <si>
-    <t>Unstructured_triangles</t>
-  </si>
-  <si>
-    <t>[0.0335583911027002, 0.0020587067645353673, 0.0003290517629436336, 8.22507622070037e-05, 2.0561929520719267e-05, 5.140434811781161e-06]</t>
-  </si>
-  <si>
     <t>squareWithSquares</t>
   </si>
   <si>
@@ -173,6 +173,33 @@
     <t>[0.0335583911027001, 0.002058706764536365, 0.000329051762941964, 8.225076224220633e-05, 2.0561929538928084e-05, 5.140434875730902e-06]</t>
   </si>
   <si>
+    <t>[0.0669509874804482, 0.06815847506446479, 0.06471965034394461, 0.06325778881561246, 0.06255657471840613, 0.06218973390644179]</t>
+  </si>
+  <si>
+    <t>[0.20788601050300354, 0.21324870454359207, 0.21369860273963248, 0.21376283055789733, 0.21377888577341903, 0.21378289946864626]</t>
+  </si>
+  <si>
+    <t>Orange(order 0)</t>
+  </si>
+  <si>
+    <t>[0.1450449320264222, 0.043301182264762685, 0.017799215386138302, 0.012676403707012044, 0.004513492486842332]</t>
+  </si>
+  <si>
+    <t>squareWithEquilateralTriangles</t>
+  </si>
+  <si>
+    <t>[u'squareWithEquilateralTriangles5', u'squareWithEquilateralTriangles20', u'squareWithEquilateralTriangles50', u'squareWithEquilateralTriangles100', u'squareWithEquilateralTriangles200']</t>
+  </si>
+  <si>
+    <t>[6.32455532033676, 26.07680962081059, 65.57438524302002, 131.14877048603998, 263.058928759318]</t>
+  </si>
+  <si>
+    <t>Structured_triangles</t>
+  </si>
+  <si>
+    <t>[0.04972168575894865, 0.04358040486275293, 0.02190713533101905, 0.011510133471144974, 0.007903217495358324]</t>
+  </si>
+  <si>
     <t>[0.03355839110270013, 0.00826541696622572, 0.0020587067645243596, 0.0009143535530931283]</t>
   </si>
   <si>
@@ -188,37 +215,10 @@
     <t>Regular_Cubes</t>
   </si>
   <si>
-    <t>[0.0669509874804482, 0.06815847506446479, 0.06471965034394461, 0.06325778881561246, 0.06255657471840613, 0.06218973390644179]</t>
-  </si>
-  <si>
-    <t>[0.20788601050300354, 0.21324870454359207, 0.21369860273963248, 0.21376283055789733, 0.21377888577341903, 0.21378289946864626]</t>
-  </si>
-  <si>
-    <t>Orange(order 0)</t>
-  </si>
-  <si>
     <t>[0.08220526266791414, 0.0844393267140037, 0.0821945418748455, 0.08112742468658361]</t>
   </si>
   <si>
     <t>[0.24690168316230734, 0.08723262076393898, 0.09807479699639379, 0.09811268005866074, 0.07589566871761519]</t>
-  </si>
-  <si>
-    <t>[0.04972168575894865, 0.04358040486275293, 0.02190713533101905, 0.011510133471144974, 0.007903217495358324]</t>
-  </si>
-  <si>
-    <t>[0.1450449320264222, 0.043301182264762685, 0.017799215386138302, 0.012676403707012044, 0.004513492486842332]</t>
-  </si>
-  <si>
-    <t>squareWithEquilateralTriangles</t>
-  </si>
-  <si>
-    <t>[u'squareWithEquilateralTriangles5', u'squareWithEquilateralTriangles20', u'squareWithEquilateralTriangles50', u'squareWithEquilateralTriangles100', u'squareWithEquilateralTriangles200']</t>
-  </si>
-  <si>
-    <t>[6.32455532033676, 26.07680962081059, 65.57438524302002, 131.14877048603998, 263.058928759318]</t>
-  </si>
-  <si>
-    <t>Structured_triangles</t>
   </si>
 </sst>
 </file>
@@ -639,7 +639,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>107.7764768600464</v>
+        <v>119.5647480487823</v>
       </c>
       <c r="C2" t="s">
         <v>19</v>
@@ -698,10 +698,10 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>208.2461259365082</v>
+        <v>6.094477891921997</v>
       </c>
       <c r="C3" t="s">
         <v>29</v>
@@ -710,25 +710,25 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" t="b">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
         <v>31</v>
       </c>
-      <c r="G3" t="n">
-        <v>2</v>
-      </c>
-      <c r="H3" t="b">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>32</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>33</v>
-      </c>
-      <c r="K3" t="s">
-        <v>34</v>
       </c>
       <c r="L3" t="s">
         <v>26</v>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="R3" t="n">
-        <v>1.340336836145038</v>
+        <v>2.015608644460145</v>
       </c>
       <c r="S3" t="n">
         <v>2</v>
@@ -760,25 +760,25 @@
     </row>
     <row r="4" spans="1:20">
       <c r="A4" s="1" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="n">
-        <v>11.92167401313782</v>
+        <v>208.4592311382294</v>
       </c>
       <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
-      </c>
-      <c r="D4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
       <c r="F4" t="s">
         <v>36</v>
       </c>
       <c r="G4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" t="b">
         <v>1</v>
@@ -811,10 +811,10 @@
         <v>1</v>
       </c>
       <c r="R4" t="n">
-        <v>0.6690820358074518</v>
+        <v>1.340336836145038</v>
       </c>
       <c r="S4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T4" t="s">
         <v>28</v>
@@ -822,10 +822,10 @@
     </row>
     <row r="5" spans="1:20">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B5" t="n">
-        <v>6.384788036346436</v>
+        <v>11.90931582450867</v>
       </c>
       <c r="C5" t="s">
         <v>40</v>
@@ -834,25 +834,25 @@
         <v>20</v>
       </c>
       <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
         <v>41</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="n">
+        <v>3</v>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
         <v>42</v>
       </c>
-      <c r="G5" t="n">
-        <v>2</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>43</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>44</v>
-      </c>
-      <c r="K5" t="s">
-        <v>45</v>
       </c>
       <c r="L5" t="s">
         <v>26</v>
@@ -873,10 +873,10 @@
         <v>1</v>
       </c>
       <c r="R5" t="n">
-        <v>2.015608644460145</v>
+        <v>0.6690820358074518</v>
       </c>
       <c r="S5" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T5" t="s">
         <v>28</v>
@@ -887,16 +887,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="n">
-        <v>10.83429408073425</v>
+        <v>9.851321935653687</v>
       </c>
       <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
         <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" t="s">
-        <v>41</v>
       </c>
       <c r="F6" t="s">
         <v>47</v>
@@ -949,7 +949,7 @@
         <v>11</v>
       </c>
       <c r="B7" t="n">
-        <v>11.39564800262451</v>
+        <v>9.898462057113647</v>
       </c>
       <c r="C7" t="s">
         <v>51</v>
@@ -958,7 +958,7 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="F7" t="s">
         <v>47</v>
@@ -1008,10 +1008,10 @@
     </row>
     <row r="8" spans="1:20">
       <c r="A8" s="1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B8" t="n">
-        <v>5.916706800460815</v>
+        <v>15.68182492256165</v>
       </c>
       <c r="C8" t="s">
         <v>52</v>
@@ -1020,10 +1020,10 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>53</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>54</v>
+        <v>22</v>
       </c>
       <c r="G8" t="n">
         <v>2</v>
@@ -1032,13 +1032,13 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J8" t="s">
-        <v>55</v>
+        <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="L8" t="s">
         <v>50</v>
@@ -1059,7 +1059,7 @@
         <v>1</v>
       </c>
       <c r="R8" t="n">
-        <v>1.340336836132099</v>
+        <v>0.02119663100406134</v>
       </c>
       <c r="S8" t="n">
         <v>2</v>
@@ -1070,13 +1070,13 @@
     </row>
     <row r="9" spans="1:20">
       <c r="A9" s="1" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B9" t="n">
-        <v>16.73147892951965</v>
+        <v>15.86531114578247</v>
       </c>
       <c r="C9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
         <v>20</v>
@@ -1121,24 +1121,24 @@
         <v>1</v>
       </c>
       <c r="R9" t="n">
-        <v>0.02119663100406134</v>
+        <v>-0.005617740418916485</v>
       </c>
       <c r="S9" t="n">
         <v>2</v>
       </c>
       <c r="T9" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:20">
       <c r="A10" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B10" t="n">
-        <v>16.02867984771729</v>
+        <v>4.744688034057617</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D10" t="s">
         <v>20</v>
@@ -1147,7 +1147,7 @@
         <v>21</v>
       </c>
       <c r="F10" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="G10" t="n">
         <v>2</v>
@@ -1156,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="J10" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="L10" t="s">
         <v>50</v>
@@ -1183,21 +1183,21 @@
         <v>1</v>
       </c>
       <c r="R10" t="n">
-        <v>-0.005617740418916485</v>
+        <v>0.8952237869134417</v>
       </c>
       <c r="S10" t="n">
         <v>2</v>
       </c>
       <c r="T10" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:20">
       <c r="A11" s="1" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="n">
-        <v>62.7276930809021</v>
+        <v>2.505467891693115</v>
       </c>
       <c r="C11" t="s">
         <v>60</v>
@@ -1206,25 +1206,25 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="n">
+        <v>2</v>
+      </c>
+      <c r="H11" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
         <v>31</v>
       </c>
-      <c r="G11" t="n">
-        <v>2</v>
-      </c>
-      <c r="H11" t="b">
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>32</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>33</v>
-      </c>
-      <c r="K11" t="s">
-        <v>34</v>
       </c>
       <c r="L11" t="s">
         <v>50</v>
@@ -1245,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="R11" t="n">
-        <v>0.006535470643459771</v>
+        <v>0.6137798580984465</v>
       </c>
       <c r="S11" t="n">
         <v>2</v>
@@ -1256,10 +1256,10 @@
     </row>
     <row r="12" spans="1:20">
       <c r="A12" s="1" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>3.762717962265015</v>
+        <v>5.868787050247192</v>
       </c>
       <c r="C12" t="s">
         <v>61</v>
@@ -1268,13 +1268,13 @@
         <v>20</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="G12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H12" t="b">
         <v>1</v>
@@ -1283,10 +1283,10 @@
         <v>37</v>
       </c>
       <c r="J12" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
       <c r="K12" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="L12" t="s">
         <v>50</v>
@@ -1307,10 +1307,10 @@
         <v>1</v>
       </c>
       <c r="R12" t="n">
-        <v>0.5358788100873692</v>
+        <v>1.340336836132099</v>
       </c>
       <c r="S12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T12" t="s">
         <v>28</v>
@@ -1318,37 +1318,37 @@
     </row>
     <row r="13" spans="1:20">
       <c r="A13" s="1" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>2.942996978759766</v>
+        <v>62.12639307975769</v>
       </c>
       <c r="C13" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="G13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13" t="b">
         <v>1</v>
       </c>
       <c r="I13" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="J13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="K13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L13" t="s">
         <v>50</v>
@@ -1369,10 +1369,10 @@
         <v>1</v>
       </c>
       <c r="R13" t="n">
-        <v>0.6137798580984465</v>
+        <v>0.006535470643459771</v>
       </c>
       <c r="S13" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T13" t="s">
         <v>28</v>
@@ -1380,39 +1380,41 @@
     </row>
     <row r="14" spans="1:20">
       <c r="A14" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>6.52453088760376</v>
+        <v>3.679362773895264</v>
       </c>
       <c r="C14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D14" t="s">
         <v>20</v>
       </c>
       <c r="E14" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" t="s">
         <v>41</v>
       </c>
-      <c r="F14" t="s">
-        <v>64</v>
-      </c>
       <c r="G14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14" t="b">
         <v>1</v>
       </c>
       <c r="I14" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="J14" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="K14" t="s">
-        <v>67</v>
-      </c>
-      <c r="L14" t="s"/>
+        <v>44</v>
+      </c>
+      <c r="L14" t="s">
+        <v>50</v>
+      </c>
       <c r="M14" t="s">
         <v>20</v>
       </c>
@@ -1429,10 +1431,10 @@
         <v>1</v>
       </c>
       <c r="R14" t="n">
-        <v>0.8952237869134417</v>
+        <v>0.5358788100873692</v>
       </c>
       <c r="S14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T14" t="s">
         <v>28</v>

</xml_diff>

<commit_message>
Updated convergence table with correction of the Equilateral mesh method
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
   <si>
     <t>Bound_cond</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Num_method</t>
   </si>
   <si>
-    <t>Num_methode</t>
-  </si>
-  <si>
     <t>Numerical_method_time_discretization</t>
   </si>
   <si>
@@ -200,6 +197,21 @@
     <t>Orange(order 0)</t>
   </si>
   <si>
+    <t>[0.1450449320264222, 0.043301182264762685, 0.017799215386138302, 0.012676403707012044, 0.004513492486842332]</t>
+  </si>
+  <si>
+    <t>squareWithEquilateralTriangles</t>
+  </si>
+  <si>
+    <t>[u'squareWithEquilateralTriangles5', u'squareWithEquilateralTriangles20', u'squareWithEquilateralTriangles50', u'squareWithEquilateralTriangles100', u'squareWithEquilateralTriangles200']</t>
+  </si>
+  <si>
+    <t>[6.32455532033676, 26.07680962081059, 65.57438524302002, 131.14877048603998, 263.058928759318]</t>
+  </si>
+  <si>
+    <t>Structured_triangles</t>
+  </si>
+  <si>
     <t>[0.04972168575894865, 0.04358040486275293, 0.02190713533101905, 0.011510133471144974, 0.007903217495358324]</t>
   </si>
   <si>
@@ -222,21 +234,6 @@
   </si>
   <si>
     <t>[0.24690168316230734, 0.08723262076393898, 0.09807479699639379, 0.09811268005866074, 0.07589566871761519]</t>
-  </si>
-  <si>
-    <t>[0.1450449320264222, 0.043301182264762685, 0.017799215386138302, 0.012676403707012044, 0.004513492486842332]</t>
-  </si>
-  <si>
-    <t>squareWithEquilateralTriangles</t>
-  </si>
-  <si>
-    <t>[u'squareWithEquilateralTriangles5', u'squareWithEquilateralTriangles20', u'squareWithEquilateralTriangles50', u'squareWithEquilateralTriangles100', u'squareWithEquilateralTriangles200']</t>
-  </si>
-  <si>
-    <t>[6.32455532033676, 26.07680962081059, 65.57438524302002, 131.14877048603998, 263.058928759318]</t>
-  </si>
-  <si>
-    <t>Structured_triangles</t>
   </si>
 </sst>
 </file>
@@ -585,7 +582,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -593,7 +590,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:23">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,168 +657,163 @@
       <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24">
-      <c r="A2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
       </c>
       <c r="C2" t="s"/>
       <c r="D2" t="n">
         <v>108.1455399990082</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="s">
         <v>27</v>
       </c>
-      <c r="I2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>28</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>29</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>30</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
         <v>31</v>
       </c>
-      <c r="O2" t="s"/>
-      <c r="P2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" t="b">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="R2" t="b">
+        <v>0</v>
+      </c>
+      <c r="S2" t="b">
+        <v>1</v>
+      </c>
+      <c r="T2" t="n">
+        <v>2.0039</v>
+      </c>
+      <c r="U2" t="n">
+        <v>2</v>
+      </c>
+      <c r="V2" t="s"/>
+      <c r="W2" t="s">
         <v>32</v>
       </c>
-      <c r="S2" t="b">
-        <v>0</v>
-      </c>
-      <c r="T2" t="b">
-        <v>1</v>
-      </c>
-      <c r="U2" t="n">
-        <v>2.0039</v>
-      </c>
-      <c r="V2" t="n">
-        <v>2</v>
-      </c>
-      <c r="W2" t="s"/>
-      <c r="X2" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:23">
       <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s"/>
       <c r="D3" t="n">
         <v>6.762243032455444</v>
       </c>
       <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" t="s">
         <v>34</v>
       </c>
-      <c r="F3" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="n">
+        <v>2</v>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
         <v>35</v>
       </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
-      </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>36</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>37</v>
       </c>
-      <c r="M3" t="s">
-        <v>38</v>
-      </c>
       <c r="N3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
         <v>31</v>
       </c>
-      <c r="O3" t="s"/>
-      <c r="P3" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q3" t="b">
-        <v>1</v>
-      </c>
-      <c r="R3" t="s">
+      <c r="R3" t="b">
+        <v>0</v>
+      </c>
+      <c r="S3" t="b">
+        <v>1</v>
+      </c>
+      <c r="T3" t="n">
+        <v>2.0156</v>
+      </c>
+      <c r="U3" t="n">
+        <v>2</v>
+      </c>
+      <c r="V3" t="s"/>
+      <c r="W3" t="s">
         <v>32</v>
       </c>
-      <c r="S3" t="b">
-        <v>0</v>
-      </c>
-      <c r="T3" t="b">
-        <v>1</v>
-      </c>
-      <c r="U3" t="n">
-        <v>2.0156</v>
-      </c>
-      <c r="V3" t="n">
-        <v>2</v>
-      </c>
-      <c r="W3" t="s"/>
-      <c r="X3" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:23">
       <c r="A4" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s"/>
       <c r="D4" t="n">
         <v>210.4683861732483</v>
       </c>
       <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>40</v>
-      </c>
-      <c r="H4" t="s">
-        <v>41</v>
       </c>
       <c r="I4" t="n">
         <v>3</v>
@@ -830,66 +822,65 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" t="s">
         <v>42</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>43</v>
       </c>
-      <c r="M4" t="s">
-        <v>44</v>
-      </c>
       <c r="N4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" t="s">
+        <v>24</v>
+      </c>
+      <c r="P4" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
         <v>31</v>
       </c>
-      <c r="O4" t="s"/>
-      <c r="P4" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q4" t="b">
-        <v>1</v>
-      </c>
-      <c r="R4" t="s">
+      <c r="R4" t="b">
+        <v>0</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" t="n">
+        <v>1.3403</v>
+      </c>
+      <c r="U4" t="n">
+        <v>3</v>
+      </c>
+      <c r="V4" t="s"/>
+      <c r="W4" t="s">
         <v>32</v>
       </c>
-      <c r="S4" t="b">
-        <v>0</v>
-      </c>
-      <c r="T4" t="b">
-        <v>1</v>
-      </c>
-      <c r="U4" t="n">
-        <v>1.3403</v>
-      </c>
-      <c r="V4" t="n">
-        <v>3</v>
-      </c>
-      <c r="W4" t="s"/>
-      <c r="X4" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:23">
       <c r="A5" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s"/>
       <c r="D5" t="n">
         <v>11.9149010181427</v>
       </c>
       <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
         <v>45</v>
-      </c>
-      <c r="F5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>46</v>
       </c>
       <c r="I5" t="n">
         <v>3</v>
@@ -898,474 +889,467 @@
         <v>1</v>
       </c>
       <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
         <v>47</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>48</v>
       </c>
-      <c r="M5" t="s">
-        <v>49</v>
-      </c>
       <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
         <v>31</v>
       </c>
-      <c r="O5" t="s"/>
-      <c r="P5" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" t="s">
+      <c r="R5" t="b">
+        <v>0</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.6691</v>
+      </c>
+      <c r="U5" t="n">
+        <v>3</v>
+      </c>
+      <c r="V5" t="s"/>
+      <c r="W5" t="s">
         <v>32</v>
       </c>
-      <c r="S5" t="b">
-        <v>0</v>
-      </c>
-      <c r="T5" t="b">
-        <v>1</v>
-      </c>
-      <c r="U5" t="n">
-        <v>0.6691</v>
-      </c>
-      <c r="V5" t="n">
-        <v>3</v>
-      </c>
-      <c r="W5" t="s"/>
-      <c r="X5" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:23">
       <c r="A6" s="1" t="n">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C6" t="s"/>
       <c r="D6" t="n">
         <v>9.832487106323242</v>
       </c>
       <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>51</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="n">
+        <v>2</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
         <v>52</v>
       </c>
-      <c r="I6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>53</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>54</v>
       </c>
-      <c r="N6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" t="s"/>
-      <c r="P6" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" t="s">
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>31</v>
+      </c>
+      <c r="R6" t="b">
+        <v>0</v>
+      </c>
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" t="n">
+        <v>2.0039</v>
+      </c>
+      <c r="U6" t="n">
+        <v>2</v>
+      </c>
+      <c r="V6" t="s"/>
+      <c r="W6" t="s">
         <v>32</v>
       </c>
-      <c r="S6" t="b">
-        <v>0</v>
-      </c>
-      <c r="T6" t="b">
-        <v>1</v>
-      </c>
-      <c r="U6" t="n">
-        <v>2.0039</v>
-      </c>
-      <c r="V6" t="n">
-        <v>2</v>
-      </c>
-      <c r="W6" t="s"/>
-      <c r="X6" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:23">
       <c r="A7" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s"/>
       <c r="D7" t="n">
         <v>9.859630107879639</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
+        <v>50</v>
+      </c>
+      <c r="H7" t="s">
         <v>51</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
         <v>52</v>
       </c>
-      <c r="I7" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>28</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>53</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>54</v>
       </c>
-      <c r="N7" t="s">
-        <v>55</v>
-      </c>
-      <c r="O7" t="s"/>
-      <c r="P7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q7" t="b">
-        <v>1</v>
-      </c>
-      <c r="R7" t="s">
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P7" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>31</v>
+      </c>
+      <c r="R7" t="b">
+        <v>0</v>
+      </c>
+      <c r="S7" t="b">
+        <v>1</v>
+      </c>
+      <c r="T7" t="n">
+        <v>2.0039</v>
+      </c>
+      <c r="U7" t="n">
+        <v>2</v>
+      </c>
+      <c r="V7" t="s"/>
+      <c r="W7" t="s">
         <v>32</v>
       </c>
-      <c r="S7" t="b">
-        <v>0</v>
-      </c>
-      <c r="T7" t="b">
-        <v>1</v>
-      </c>
-      <c r="U7" t="n">
-        <v>2.0039</v>
-      </c>
-      <c r="V7" t="n">
-        <v>2</v>
-      </c>
-      <c r="W7" t="s"/>
-      <c r="X7" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:23">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s"/>
       <c r="D8" t="n">
         <v>15.65501999855042</v>
       </c>
       <c r="E8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="n">
+        <v>2</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
         <v>27</v>
       </c>
-      <c r="I8" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>28</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>29</v>
       </c>
-      <c r="M8" t="s">
-        <v>30</v>
-      </c>
       <c r="N8" t="s">
-        <v>55</v>
-      </c>
-      <c r="O8" t="s"/>
-      <c r="P8" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q8" t="b">
-        <v>1</v>
-      </c>
-      <c r="R8" t="s">
+        <v>54</v>
+      </c>
+      <c r="O8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" t="b">
+        <v>0</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.0212</v>
+      </c>
+      <c r="U8" t="n">
+        <v>2</v>
+      </c>
+      <c r="V8" t="s"/>
+      <c r="W8" t="s">
         <v>32</v>
       </c>
-      <c r="S8" t="b">
-        <v>0</v>
-      </c>
-      <c r="T8" t="b">
-        <v>1</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0.0212</v>
-      </c>
-      <c r="V8" t="n">
-        <v>2</v>
-      </c>
-      <c r="W8" t="s"/>
-      <c r="X8" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:23">
       <c r="A9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s"/>
       <c r="D9" t="n">
         <v>15.78992199897766</v>
       </c>
       <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N9" t="s">
+        <v>54</v>
+      </c>
+      <c r="O9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>31</v>
+      </c>
+      <c r="R9" t="b">
+        <v>0</v>
+      </c>
+      <c r="S9" t="b">
+        <v>1</v>
+      </c>
+      <c r="T9" t="n">
+        <v>-0.0056</v>
+      </c>
+      <c r="U9" t="n">
+        <v>2</v>
+      </c>
+      <c r="V9" t="s"/>
+      <c r="W9" t="s">
         <v>59</v>
       </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" t="b">
-        <v>1</v>
-      </c>
-      <c r="K9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L9" t="s">
-        <v>29</v>
-      </c>
-      <c r="M9" t="s">
-        <v>30</v>
-      </c>
-      <c r="N9" t="s">
-        <v>55</v>
-      </c>
-      <c r="O9" t="s"/>
-      <c r="P9" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q9" t="b">
-        <v>1</v>
-      </c>
-      <c r="R9" t="s">
-        <v>32</v>
-      </c>
-      <c r="S9" t="b">
-        <v>0</v>
-      </c>
-      <c r="T9" t="b">
-        <v>1</v>
-      </c>
-      <c r="U9" t="n">
-        <v>-0.0056</v>
-      </c>
-      <c r="V9" t="n">
-        <v>2</v>
-      </c>
-      <c r="W9" t="s"/>
-      <c r="X9" t="s">
-        <v>60</v>
-      </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:23">
       <c r="A10" s="1" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s"/>
       <c r="D10" t="n">
+        <v>4.86047887802124</v>
+      </c>
+      <c r="E10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>61</v>
+      </c>
+      <c r="I10" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>62</v>
+      </c>
+      <c r="L10" t="s">
+        <v>63</v>
+      </c>
+      <c r="M10" t="s">
+        <v>64</v>
+      </c>
+      <c r="N10" t="s">
+        <v>54</v>
+      </c>
+      <c r="O10" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>31</v>
+      </c>
+      <c r="R10" t="b">
+        <v>0</v>
+      </c>
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.8952</v>
+      </c>
+      <c r="U10" t="n">
+        <v>2</v>
+      </c>
+      <c r="V10" t="s"/>
+      <c r="W10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23">
+      <c r="A11" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s"/>
+      <c r="D11" t="n">
         <v>2.600184917449951</v>
       </c>
-      <c r="E10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" t="s">
+      <c r="E11" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
         <v>25</v>
       </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
         <v>35</v>
       </c>
-      <c r="I10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" t="b">
-        <v>1</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="L11" t="s">
         <v>36</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M11" t="s">
         <v>37</v>
       </c>
-      <c r="M10" t="s">
-        <v>38</v>
-      </c>
-      <c r="N10" t="s">
-        <v>55</v>
-      </c>
-      <c r="O10" t="s"/>
-      <c r="P10" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R10" t="s">
+      <c r="N11" t="s">
+        <v>54</v>
+      </c>
+      <c r="O11" t="s">
+        <v>24</v>
+      </c>
+      <c r="P11" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>31</v>
+      </c>
+      <c r="R11" t="b">
+        <v>0</v>
+      </c>
+      <c r="S11" t="b">
+        <v>1</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.6138</v>
+      </c>
+      <c r="U11" t="n">
+        <v>2</v>
+      </c>
+      <c r="V11" t="s"/>
+      <c r="W11" t="s">
         <v>32</v>
       </c>
-      <c r="S10" t="b">
-        <v>0</v>
-      </c>
-      <c r="T10" t="b">
-        <v>1</v>
-      </c>
-      <c r="U10" t="n">
-        <v>0.6138</v>
-      </c>
-      <c r="V10" t="n">
-        <v>2</v>
-      </c>
-      <c r="W10" t="s"/>
-      <c r="X10" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="11" spans="1:24">
-      <c r="A11" s="1" t="n">
+    <row r="12" spans="1:23">
+      <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="s"/>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="n">
+      <c r="B12" t="s"/>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="n">
         <v>5.900697946548462</v>
       </c>
-      <c r="E11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" t="s">
-        <v>63</v>
-      </c>
-      <c r="H11" t="s">
-        <v>64</v>
-      </c>
-      <c r="I11" t="n">
-        <v>3</v>
-      </c>
-      <c r="J11" t="b">
-        <v>1</v>
-      </c>
-      <c r="K11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L11" t="s">
-        <v>65</v>
-      </c>
-      <c r="M11" t="s">
+      <c r="E12" t="s">
         <v>66</v>
       </c>
-      <c r="N11" t="s">
-        <v>55</v>
-      </c>
-      <c r="O11" t="s"/>
-      <c r="P11" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q11" t="b">
-        <v>1</v>
-      </c>
-      <c r="R11" t="s">
-        <v>32</v>
-      </c>
-      <c r="S11" t="b">
-        <v>0</v>
-      </c>
-      <c r="T11" t="b">
-        <v>1</v>
-      </c>
-      <c r="U11" t="n">
-        <v>1.3403</v>
-      </c>
-      <c r="V11" t="n">
-        <v>3</v>
-      </c>
-      <c r="W11" t="s"/>
-      <c r="X11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:24">
-      <c r="A12" s="1" t="n">
-        <v>9</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" t="s"/>
-      <c r="D12" t="n">
-        <v>62.56098890304565</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
         <v>67</v>
       </c>
-      <c r="F12" t="s">
-        <v>25</v>
-      </c>
-      <c r="G12" t="s">
-        <v>40</v>
-      </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>68</v>
       </c>
       <c r="I12" t="n">
         <v>3</v>
@@ -1374,66 +1358,65 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L12" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="M12" t="s">
-        <v>44</v>
+        <v>70</v>
       </c>
       <c r="N12" t="s">
-        <v>55</v>
-      </c>
-      <c r="O12" t="s"/>
-      <c r="P12" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q12" t="b">
-        <v>1</v>
-      </c>
-      <c r="R12" t="s">
+        <v>54</v>
+      </c>
+      <c r="O12" t="s">
+        <v>24</v>
+      </c>
+      <c r="P12" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" t="b">
+        <v>0</v>
+      </c>
+      <c r="S12" t="b">
+        <v>1</v>
+      </c>
+      <c r="T12" t="n">
+        <v>1.3403</v>
+      </c>
+      <c r="U12" t="n">
+        <v>3</v>
+      </c>
+      <c r="V12" t="s"/>
+      <c r="W12" t="s">
         <v>32</v>
       </c>
-      <c r="S12" t="b">
-        <v>0</v>
-      </c>
-      <c r="T12" t="b">
-        <v>1</v>
-      </c>
-      <c r="U12" t="n">
-        <v>0.0065</v>
-      </c>
-      <c r="V12" t="s"/>
-      <c r="W12" t="n">
-        <v>3</v>
-      </c>
-      <c r="X12" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:23">
       <c r="A13" s="1" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s"/>
       <c r="D13" t="n">
-        <v>3.782500028610229</v>
+        <v>62.56098890304565</v>
       </c>
       <c r="E13" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
+        <v>39</v>
+      </c>
+      <c r="H13" t="s">
         <v>40</v>
-      </c>
-      <c r="H13" t="s">
-        <v>46</v>
       </c>
       <c r="I13" t="n">
         <v>3</v>
@@ -1442,110 +1425,108 @@
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="L13" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="M13" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="N13" t="s">
-        <v>55</v>
-      </c>
-      <c r="O13" t="s"/>
-      <c r="P13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q13" t="b">
-        <v>1</v>
-      </c>
-      <c r="R13" t="s">
-        <v>32</v>
+        <v>54</v>
+      </c>
+      <c r="O13" t="s">
+        <v>24</v>
+      </c>
+      <c r="P13" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>31</v>
+      </c>
+      <c r="R13" t="b">
+        <v>0</v>
       </c>
       <c r="S13" t="b">
-        <v>0</v>
-      </c>
-      <c r="T13" t="b">
-        <v>1</v>
-      </c>
-      <c r="U13" t="n">
-        <v>0.5359</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="U13" t="s"/>
       <c r="V13" t="n">
         <v>3</v>
       </c>
-      <c r="W13" t="s"/>
-      <c r="X13" t="s">
-        <v>33</v>
+      <c r="W13" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:23">
       <c r="A14" s="1" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C14" t="s"/>
       <c r="D14" t="n">
-        <v>4.790747165679932</v>
+        <v>3.782500028610229</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="H14" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="I14" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="L14" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="M14" t="s">
-        <v>73</v>
-      </c>
-      <c r="N14" t="s"/>
+        <v>48</v>
+      </c>
+      <c r="N14" t="s">
+        <v>54</v>
+      </c>
       <c r="O14" t="s">
-        <v>55</v>
-      </c>
-      <c r="P14" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q14" t="b">
-        <v>1</v>
-      </c>
-      <c r="R14" t="s">
+        <v>24</v>
+      </c>
+      <c r="P14" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>31</v>
+      </c>
+      <c r="R14" t="b">
+        <v>0</v>
+      </c>
+      <c r="S14" t="b">
+        <v>1</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.5359</v>
+      </c>
+      <c r="U14" t="n">
+        <v>3</v>
+      </c>
+      <c r="V14" t="s"/>
+      <c r="W14" t="s">
         <v>32</v>
-      </c>
-      <c r="S14" t="b">
-        <v>0</v>
-      </c>
-      <c r="T14" t="b">
-        <v>1</v>
-      </c>
-      <c r="U14" t="n">
-        <v>0.8952</v>
-      </c>
-      <c r="V14" t="n">
-        <v>2</v>
-      </c>
-      <c r="W14" t="s"/>
-      <c r="X14" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated convergence table with rounding of the computational time
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
@@ -15,12 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
   <si>
     <t>Bound_cond</t>
-  </si>
-  <si>
-    <t>Bound_condn</t>
   </si>
   <si>
     <t>Comput_time</t>
@@ -582,7 +579,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:W14"/>
+  <dimension ref="A1:V14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -590,7 +587,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:22">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -654,20 +651,19 @@
       <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
-      <c r="A2" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="n">
+        <v>105.362</v>
+      </c>
+      <c r="D2" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" t="s"/>
-      <c r="D2" t="n">
-        <v>108.1455399990082</v>
       </c>
       <c r="E2" t="s">
         <v>23</v>
@@ -678,14 +674,14 @@
       <c r="G2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" t="b">
-        <v>1</v>
       </c>
       <c r="K2" t="s">
         <v>27</v>
@@ -697,62 +693,61 @@
         <v>29</v>
       </c>
       <c r="N2" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
         <v>30</v>
       </c>
-      <c r="O2" t="s">
-        <v>24</v>
-      </c>
-      <c r="P2" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="Q2" t="b">
+        <v>0</v>
+      </c>
+      <c r="R2" t="b">
+        <v>1</v>
+      </c>
+      <c r="S2" t="n">
+        <v>2.0039</v>
+      </c>
+      <c r="T2" t="n">
+        <v>2</v>
+      </c>
+      <c r="U2" t="s"/>
+      <c r="V2" t="s">
         <v>31</v>
       </c>
-      <c r="R2" t="b">
-        <v>0</v>
-      </c>
-      <c r="S2" t="b">
-        <v>1</v>
-      </c>
-      <c r="T2" t="n">
-        <v>2.0039</v>
-      </c>
-      <c r="U2" t="n">
-        <v>2</v>
-      </c>
-      <c r="V2" t="s"/>
-      <c r="W2" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:22">
       <c r="A3" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s"/>
-      <c r="D3" t="n">
-        <v>6.762243032455444</v>
+        <v>21</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F3" t="s">
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" t="b">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
         <v>34</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2</v>
-      </c>
-      <c r="J3" t="b">
-        <v>1</v>
       </c>
       <c r="K3" t="s">
         <v>35</v>
@@ -761,65 +756,64 @@
         <v>36</v>
       </c>
       <c r="M3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="N3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O3" t="b">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
         <v>30</v>
       </c>
-      <c r="O3" t="s">
-        <v>24</v>
-      </c>
-      <c r="P3" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="Q3" t="b">
+        <v>0</v>
+      </c>
+      <c r="R3" t="b">
+        <v>1</v>
+      </c>
+      <c r="S3" t="n">
+        <v>2.0156</v>
+      </c>
+      <c r="T3" t="n">
+        <v>2</v>
+      </c>
+      <c r="U3" t="s"/>
+      <c r="V3" t="s">
         <v>31</v>
       </c>
-      <c r="R3" t="b">
-        <v>0</v>
-      </c>
-      <c r="S3" t="b">
-        <v>1</v>
-      </c>
-      <c r="T3" t="n">
-        <v>2.0156</v>
-      </c>
-      <c r="U3" t="n">
-        <v>2</v>
-      </c>
-      <c r="V3" t="s"/>
-      <c r="W3" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:22">
       <c r="A4" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s"/>
-      <c r="D4" t="n">
-        <v>210.4683861732483</v>
+        <v>21</v>
+      </c>
+      <c r="C4" t="n">
+        <v>209.234</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
       </c>
       <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
         <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>24</v>
       </c>
       <c r="G4" t="s">
         <v>39</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>40</v>
-      </c>
-      <c r="I4" t="n">
-        <v>3</v>
-      </c>
-      <c r="J4" t="b">
-        <v>1</v>
       </c>
       <c r="K4" t="s">
         <v>41</v>
@@ -828,65 +822,64 @@
         <v>42</v>
       </c>
       <c r="M4" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="N4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O4" t="b">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
         <v>30</v>
       </c>
-      <c r="O4" t="s">
-        <v>24</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="Q4" t="b">
+        <v>0</v>
+      </c>
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>1.3403</v>
+      </c>
+      <c r="T4" t="n">
+        <v>3</v>
+      </c>
+      <c r="U4" t="s"/>
+      <c r="V4" t="s">
         <v>31</v>
       </c>
-      <c r="R4" t="b">
-        <v>0</v>
-      </c>
-      <c r="S4" t="b">
-        <v>1</v>
-      </c>
-      <c r="T4" t="n">
-        <v>1.3403</v>
-      </c>
-      <c r="U4" t="n">
-        <v>3</v>
-      </c>
-      <c r="V4" t="s"/>
-      <c r="W4" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="5" spans="1:23">
+    <row r="5" spans="1:22">
       <c r="A5" s="1" t="n">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s"/>
-      <c r="D5" t="n">
-        <v>11.9149010181427</v>
+        <v>21</v>
+      </c>
+      <c r="C5" t="n">
+        <v>11.911</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
       </c>
       <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" t="s">
         <v>44</v>
       </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" t="s">
-        <v>39</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
         <v>45</v>
-      </c>
-      <c r="I5" t="n">
-        <v>3</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
       </c>
       <c r="K5" t="s">
         <v>46</v>
@@ -895,68 +888,67 @@
         <v>47</v>
       </c>
       <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" t="b">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" t="b">
+        <v>0</v>
+      </c>
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.6691</v>
+      </c>
+      <c r="T5" t="n">
+        <v>3</v>
+      </c>
+      <c r="U5" t="s"/>
+      <c r="V5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9.772</v>
+      </c>
+      <c r="D6" t="s">
         <v>48</v>
       </c>
-      <c r="N5" t="s">
-        <v>30</v>
-      </c>
-      <c r="O5" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>31</v>
-      </c>
-      <c r="R5" t="b">
-        <v>0</v>
-      </c>
-      <c r="S5" t="b">
-        <v>1</v>
-      </c>
-      <c r="T5" t="n">
-        <v>0.6691</v>
-      </c>
-      <c r="U5" t="n">
-        <v>3</v>
-      </c>
-      <c r="V5" t="s"/>
-      <c r="W5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23">
-      <c r="A6" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s"/>
-      <c r="D6" t="n">
-        <v>9.832487106323242</v>
-      </c>
       <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
         <v>49</v>
-      </c>
-      <c r="F6" t="s">
-        <v>24</v>
       </c>
       <c r="G6" t="s">
         <v>50</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="s">
         <v>51</v>
-      </c>
-      <c r="I6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="s">
-        <v>27</v>
       </c>
       <c r="L6" t="s">
         <v>52</v>
@@ -965,65 +957,64 @@
         <v>53</v>
       </c>
       <c r="N6" t="s">
-        <v>54</v>
-      </c>
-      <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q6" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" t="b">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q6" t="b">
+        <v>0</v>
+      </c>
+      <c r="R6" t="b">
+        <v>1</v>
+      </c>
+      <c r="S6" t="n">
+        <v>2.0039</v>
+      </c>
+      <c r="T6" t="n">
+        <v>2</v>
+      </c>
+      <c r="U6" t="s"/>
+      <c r="V6" t="s">
         <v>31</v>
       </c>
-      <c r="R6" t="b">
-        <v>0</v>
-      </c>
-      <c r="S6" t="b">
-        <v>1</v>
-      </c>
-      <c r="T6" t="n">
-        <v>2.0039</v>
-      </c>
-      <c r="U6" t="n">
-        <v>2</v>
-      </c>
-      <c r="V6" t="s"/>
-      <c r="W6" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:22">
       <c r="A7" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="n">
+        <v>9.846</v>
+      </c>
+      <c r="D7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" t="s"/>
-      <c r="D7" t="n">
-        <v>9.859630107879639</v>
-      </c>
       <c r="E7" t="s">
-        <v>56</v>
+        <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>49</v>
       </c>
       <c r="G7" t="s">
         <v>50</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" t="s">
         <v>51</v>
-      </c>
-      <c r="I7" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" t="b">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
-        <v>27</v>
       </c>
       <c r="L7" t="s">
         <v>52</v>
@@ -1032,47 +1023,46 @@
         <v>53</v>
       </c>
       <c r="N7" t="s">
-        <v>54</v>
-      </c>
-      <c r="O7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P7" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O7" t="b">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" t="b">
+        <v>0</v>
+      </c>
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" t="n">
+        <v>2.0039</v>
+      </c>
+      <c r="T7" t="n">
+        <v>2</v>
+      </c>
+      <c r="U7" t="s"/>
+      <c r="V7" t="s">
         <v>31</v>
       </c>
-      <c r="R7" t="b">
-        <v>0</v>
-      </c>
-      <c r="S7" t="b">
-        <v>1</v>
-      </c>
-      <c r="T7" t="n">
-        <v>2.0039</v>
-      </c>
-      <c r="U7" t="n">
-        <v>2</v>
-      </c>
-      <c r="V7" t="s"/>
-      <c r="W7" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:22">
       <c r="A8" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s"/>
-      <c r="D8" t="n">
-        <v>15.65501999855042</v>
+        <v>21</v>
+      </c>
+      <c r="C8" t="n">
+        <v>15.677</v>
+      </c>
+      <c r="D8" t="s">
+        <v>56</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
         <v>24</v>
@@ -1080,14 +1070,14 @@
       <c r="G8" t="s">
         <v>25</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
         <v>26</v>
-      </c>
-      <c r="I8" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" t="b">
-        <v>1</v>
       </c>
       <c r="K8" t="s">
         <v>27</v>
@@ -1096,50 +1086,49 @@
         <v>28</v>
       </c>
       <c r="M8" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="N8" t="s">
-        <v>54</v>
-      </c>
-      <c r="O8" t="s">
-        <v>24</v>
-      </c>
-      <c r="P8" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q8" t="s">
+        <v>23</v>
+      </c>
+      <c r="O8" t="b">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q8" t="b">
+        <v>0</v>
+      </c>
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.0212</v>
+      </c>
+      <c r="T8" t="n">
+        <v>2</v>
+      </c>
+      <c r="U8" t="s"/>
+      <c r="V8" t="s">
         <v>31</v>
       </c>
-      <c r="R8" t="b">
-        <v>0</v>
-      </c>
-      <c r="S8" t="b">
-        <v>1</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0.0212</v>
-      </c>
-      <c r="U8" t="n">
-        <v>2</v>
-      </c>
-      <c r="V8" t="s"/>
-      <c r="W8" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:22">
       <c r="A9" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" t="s"/>
-      <c r="D9" t="n">
-        <v>15.78992199897766</v>
+        <v>54</v>
+      </c>
+      <c r="C9" t="n">
+        <v>15.956</v>
+      </c>
+      <c r="D9" t="s">
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>58</v>
+        <v>23</v>
       </c>
       <c r="F9" t="s">
         <v>24</v>
@@ -1147,14 +1136,14 @@
       <c r="G9" t="s">
         <v>25</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" t="b">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
         <v>26</v>
-      </c>
-      <c r="I9" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" t="b">
-        <v>1</v>
       </c>
       <c r="K9" t="s">
         <v>27</v>
@@ -1163,65 +1152,64 @@
         <v>28</v>
       </c>
       <c r="M9" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="N9" t="s">
-        <v>54</v>
-      </c>
-      <c r="O9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P9" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="O9" t="b">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" t="b">
+        <v>0</v>
       </c>
       <c r="R9" t="b">
-        <v>0</v>
-      </c>
-      <c r="S9" t="b">
-        <v>1</v>
+        <v>1</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-0.0056</v>
       </c>
       <c r="T9" t="n">
-        <v>-0.0056</v>
-      </c>
-      <c r="U9" t="n">
-        <v>2</v>
-      </c>
-      <c r="V9" t="s"/>
-      <c r="W9" t="s">
-        <v>59</v>
+        <v>2</v>
+      </c>
+      <c r="U9" t="s"/>
+      <c r="V9" t="s">
+        <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:22">
       <c r="A10" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" t="s"/>
-      <c r="D10" t="n">
-        <v>4.86047887802124</v>
+        <v>21</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.784</v>
+      </c>
+      <c r="D10" t="s">
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="F10" t="s">
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" t="b">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
         <v>61</v>
-      </c>
-      <c r="I10" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" t="b">
-        <v>1</v>
       </c>
       <c r="K10" t="s">
         <v>62</v>
@@ -1230,65 +1218,64 @@
         <v>63</v>
       </c>
       <c r="M10" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="N10" t="s">
-        <v>54</v>
-      </c>
-      <c r="O10" t="s">
-        <v>24</v>
-      </c>
-      <c r="P10" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q10" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" t="b">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" t="b">
+        <v>0</v>
+      </c>
+      <c r="R10" t="b">
+        <v>1</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.8952</v>
+      </c>
+      <c r="T10" t="n">
+        <v>2</v>
+      </c>
+      <c r="U10" t="s"/>
+      <c r="V10" t="s">
         <v>31</v>
       </c>
-      <c r="R10" t="b">
-        <v>0</v>
-      </c>
-      <c r="S10" t="b">
-        <v>1</v>
-      </c>
-      <c r="T10" t="n">
-        <v>0.8952</v>
-      </c>
-      <c r="U10" t="n">
-        <v>2</v>
-      </c>
-      <c r="V10" t="s"/>
-      <c r="W10" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:22">
       <c r="A11" s="1" t="n">
         <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s"/>
-      <c r="D11" t="n">
-        <v>2.600184917449951</v>
+        <v>21</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2.487</v>
+      </c>
+      <c r="D11" t="s">
+        <v>64</v>
       </c>
       <c r="E11" t="s">
-        <v>65</v>
+        <v>23</v>
       </c>
       <c r="F11" t="s">
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
-      </c>
-      <c r="H11" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
         <v>34</v>
-      </c>
-      <c r="I11" t="n">
-        <v>2</v>
-      </c>
-      <c r="J11" t="b">
-        <v>1</v>
       </c>
       <c r="K11" t="s">
         <v>35</v>
@@ -1297,132 +1284,130 @@
         <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="N11" t="s">
-        <v>54</v>
-      </c>
-      <c r="O11" t="s">
-        <v>24</v>
-      </c>
-      <c r="P11" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O11" t="b">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q11" t="b">
+        <v>0</v>
+      </c>
+      <c r="R11" t="b">
+        <v>1</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.6138</v>
+      </c>
+      <c r="T11" t="n">
+        <v>2</v>
+      </c>
+      <c r="U11" t="s"/>
+      <c r="V11" t="s">
         <v>31</v>
       </c>
-      <c r="R11" t="b">
-        <v>0</v>
-      </c>
-      <c r="S11" t="b">
-        <v>1</v>
-      </c>
-      <c r="T11" t="n">
-        <v>0.6138</v>
-      </c>
-      <c r="U11" t="n">
-        <v>2</v>
-      </c>
-      <c r="V11" t="s"/>
-      <c r="W11" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:22">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="s"/>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" t="n">
-        <v>5.900697946548462</v>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="n">
+        <v>5.976</v>
+      </c>
+      <c r="D12" t="s">
+        <v>65</v>
       </c>
       <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
         <v>66</v>
-      </c>
-      <c r="F12" t="s">
-        <v>24</v>
       </c>
       <c r="G12" t="s">
         <v>67</v>
       </c>
-      <c r="H12" t="s">
+      <c r="H12" t="n">
+        <v>3</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="s">
         <v>68</v>
-      </c>
-      <c r="I12" t="n">
-        <v>3</v>
-      </c>
-      <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="s">
-        <v>41</v>
       </c>
       <c r="L12" t="s">
         <v>69</v>
       </c>
       <c r="M12" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="N12" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" t="s">
-        <v>24</v>
-      </c>
-      <c r="P12" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q12" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" t="b">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" t="b">
+        <v>0</v>
+      </c>
+      <c r="R12" t="b">
+        <v>1</v>
+      </c>
+      <c r="S12" t="n">
+        <v>1.3403</v>
+      </c>
+      <c r="T12" t="n">
+        <v>3</v>
+      </c>
+      <c r="U12" t="s"/>
+      <c r="V12" t="s">
         <v>31</v>
       </c>
-      <c r="R12" t="b">
-        <v>0</v>
-      </c>
-      <c r="S12" t="b">
-        <v>1</v>
-      </c>
-      <c r="T12" t="n">
-        <v>1.3403</v>
-      </c>
-      <c r="U12" t="n">
-        <v>3</v>
-      </c>
-      <c r="V12" t="s"/>
-      <c r="W12" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="n">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s"/>
-      <c r="D13" t="n">
-        <v>62.56098890304565</v>
+        <v>21</v>
+      </c>
+      <c r="C13" t="n">
+        <v>62.252</v>
+      </c>
+      <c r="D13" t="s">
+        <v>70</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>23</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="G13" t="s">
         <v>39</v>
       </c>
-      <c r="H13" t="s">
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
         <v>40</v>
-      </c>
-      <c r="I13" t="n">
-        <v>3</v>
-      </c>
-      <c r="J13" t="b">
-        <v>1</v>
       </c>
       <c r="K13" t="s">
         <v>41</v>
@@ -1431,65 +1416,64 @@
         <v>42</v>
       </c>
       <c r="M13" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="N13" t="s">
-        <v>54</v>
-      </c>
-      <c r="O13" t="s">
-        <v>24</v>
-      </c>
-      <c r="P13" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O13" t="b">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q13" t="b">
+        <v>0</v>
+      </c>
+      <c r="R13" t="b">
+        <v>1</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="T13" t="s"/>
+      <c r="U13" t="n">
+        <v>3</v>
+      </c>
+      <c r="V13" t="s">
         <v>31</v>
       </c>
-      <c r="R13" t="b">
-        <v>0</v>
-      </c>
-      <c r="S13" t="b">
-        <v>1</v>
-      </c>
-      <c r="T13" t="n">
-        <v>0.0065</v>
-      </c>
-      <c r="U13" t="s"/>
-      <c r="V13" t="n">
-        <v>3</v>
-      </c>
-      <c r="W13" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:22">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" t="s"/>
-      <c r="D14" t="n">
-        <v>3.782500028610229</v>
+        <v>21</v>
+      </c>
+      <c r="C14" t="n">
+        <v>3.775</v>
+      </c>
+      <c r="D14" t="s">
+        <v>71</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="F14" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" t="b">
+        <v>1</v>
+      </c>
+      <c r="J14" t="s">
         <v>45</v>
-      </c>
-      <c r="I14" t="n">
-        <v>3</v>
-      </c>
-      <c r="J14" t="b">
-        <v>1</v>
       </c>
       <c r="K14" t="s">
         <v>46</v>
@@ -1498,35 +1482,32 @@
         <v>47</v>
       </c>
       <c r="M14" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="N14" t="s">
-        <v>54</v>
-      </c>
-      <c r="O14" t="s">
-        <v>24</v>
-      </c>
-      <c r="P14" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q14" t="s">
+        <v>23</v>
+      </c>
+      <c r="O14" t="b">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q14" t="b">
+        <v>0</v>
+      </c>
+      <c r="R14" t="b">
+        <v>1</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.5359</v>
+      </c>
+      <c r="T14" t="n">
+        <v>3</v>
+      </c>
+      <c r="U14" t="s"/>
+      <c r="V14" t="s">
         <v>31</v>
-      </c>
-      <c r="R14" t="b">
-        <v>0</v>
-      </c>
-      <c r="S14" t="b">
-        <v>1</v>
-      </c>
-      <c r="T14" t="n">
-        <v>0.5359</v>
-      </c>
-      <c r="U14" t="n">
-        <v>3</v>
-      </c>
-      <c r="V14" t="s"/>
-      <c r="W14" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Result table with new working neumann tests
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
   <si>
     <t>Bound_cond</t>
   </si>
@@ -113,6 +113,15 @@
     <t>Green</t>
   </si>
   <si>
+    <t>Neumann</t>
+  </si>
+  <si>
+    <t>[0.7503307283176518, 0.2539544973957279, 0.10870368061041591, 0.055777341080608625, 0.028297242335636467, 0.014264092354052018]</t>
+  </si>
+  <si>
+    <t>Orange (ILU)</t>
+  </si>
+  <si>
     <t>[0.17381931436989675, 0.015704630897802694, 0.0050889346986909955, 0.0008049994197372305, 0.00020964279836201426]</t>
   </si>
   <si>
@@ -128,6 +137,15 @@
     <t>Unstructured_triangles</t>
   </si>
   <si>
+    <t>[0.6631505332206331, 0.39408058878012564, 0.21896100196675858, 0.09151553643693577, 0.04861943552271186]</t>
+  </si>
+  <si>
+    <t>Squares</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
     <t>[0.033558391102700875, 0.008265416966230732, 0.0020587067645389525, 0.0009143535530498623]</t>
   </si>
   <si>
@@ -164,9 +182,6 @@
     <t>[0.0335583911027002, 0.0020587067645353673, 0.0003290517629436336, 8.22507622070037e-05, 2.0561929520719267e-05, 5.140434811781161e-06]</t>
   </si>
   <si>
-    <t>Squares</t>
-  </si>
-  <si>
     <t>squareWithSquares</t>
   </si>
   <si>
@@ -179,9 +194,6 @@
     <t>FV</t>
   </si>
   <si>
-    <t>Neumann</t>
-  </si>
-  <si>
     <t>[0.0335583911027001, 0.002058706764536365, 0.000329051762941964, 8.225076224220633e-05, 2.0561929538928084e-05, 5.140434875730902e-06]</t>
   </si>
   <si>
@@ -191,7 +203,8 @@
     <t>[0.20788601050300354, 0.21324870454359207, 0.21369860273963248, 0.21376283055789733, 0.21377888577341903, 0.21378289946864626]</t>
   </si>
   <si>
-    <t>Orange(order 0)</t>
+    <t>Orange 
+ (suspicious order 0 convergence)</t>
   </si>
   <si>
     <t>[0.1450449320264222, 0.043301182264762685, 0.017799215386138302, 0.012676403707012044, 0.004513492486842332]</t>
@@ -207,6 +220,10 @@
   </si>
   <si>
     <t>Structured_triangles</t>
+  </si>
+  <si>
+    <t>Orange 
+ (BC don't fit the domain)</t>
   </si>
   <si>
     <t>[0.04972168575894865, 0.04358040486275293, 0.02190713533101905, 0.011510133471144974, 0.007903217495358324]</t>
@@ -579,7 +596,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -660,7 +677,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="n">
-        <v>105.362</v>
+        <v>103.069</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -720,16 +737,16 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C3" t="n">
-        <v>6.3</v>
+        <v>26.158</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -738,7 +755,7 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H3" t="n">
         <v>2</v>
@@ -747,13 +764,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="L3" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M3" t="s">
         <v>29</v>
@@ -774,52 +791,52 @@
         <v>1</v>
       </c>
       <c r="S3" t="n">
-        <v>2.0156</v>
+        <v>0.9103</v>
       </c>
       <c r="T3" t="n">
         <v>2</v>
       </c>
       <c r="U3" t="s"/>
       <c r="V3" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="1" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>21</v>
       </c>
       <c r="C4" t="n">
-        <v>209.234</v>
+        <v>7.609</v>
       </c>
       <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" t="b">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="K4" t="s">
         <v>38</v>
       </c>
-      <c r="G4" t="s">
+      <c r="L4" t="s">
         <v>39</v>
-      </c>
-      <c r="H4" t="n">
-        <v>3</v>
-      </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="s">
-        <v>40</v>
-      </c>
-      <c r="K4" t="s">
-        <v>41</v>
-      </c>
-      <c r="L4" t="s">
-        <v>42</v>
       </c>
       <c r="M4" t="s">
         <v>29</v>
@@ -840,10 +857,10 @@
         <v>1</v>
       </c>
       <c r="S4" t="n">
-        <v>1.3403</v>
+        <v>2.0156</v>
       </c>
       <c r="T4" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U4" t="s"/>
       <c r="V4" t="s">
@@ -852,40 +869,40 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="1" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C5" t="n">
-        <v>11.911</v>
+        <v>3.102</v>
       </c>
       <c r="D5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E5" t="s">
         <v>23</v>
       </c>
       <c r="F5" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" t="s">
         <v>38</v>
       </c>
-      <c r="G5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H5" t="n">
-        <v>3</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-      <c r="K5" t="s">
-        <v>46</v>
-      </c>
       <c r="L5" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="M5" t="s">
         <v>29</v>
@@ -906,55 +923,55 @@
         <v>1</v>
       </c>
       <c r="S5" t="n">
-        <v>0.6691</v>
+        <v>0.8202</v>
       </c>
       <c r="T5" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U5" t="s"/>
       <c r="V5" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>9.772</v>
+        <v>208.494</v>
       </c>
       <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" t="s">
+        <v>47</v>
+      </c>
+      <c r="L6" t="s">
         <v>48</v>
       </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K6" t="s">
-        <v>51</v>
-      </c>
-      <c r="L6" t="s">
-        <v>52</v>
-      </c>
       <c r="M6" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N6" t="s">
         <v>23</v>
@@ -972,10 +989,10 @@
         <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>2.0039</v>
+        <v>1.3403</v>
       </c>
       <c r="T6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U6" t="s"/>
       <c r="V6" t="s">
@@ -984,43 +1001,43 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>9.846</v>
+        <v>12.001</v>
       </c>
       <c r="D7" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="G7" t="s">
         <v>50</v>
       </c>
       <c r="H7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="K7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="M7" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="N7" t="s">
         <v>23</v>
@@ -1038,10 +1055,10 @@
         <v>1</v>
       </c>
       <c r="S7" t="n">
-        <v>2.0039</v>
+        <v>0.6691</v>
       </c>
       <c r="T7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U7" t="s"/>
       <c r="V7" t="s">
@@ -1050,25 +1067,25 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="1" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>15.677</v>
+        <v>9.776999999999999</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
         <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="G8" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="H8" t="n">
         <v>2</v>
@@ -1080,13 +1097,13 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="M8" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
         <v>23</v>
@@ -1104,7 +1121,7 @@
         <v>1</v>
       </c>
       <c r="S8" t="n">
-        <v>0.0212</v>
+        <v>2.0039</v>
       </c>
       <c r="T8" t="n">
         <v>2</v>
@@ -1116,25 +1133,25 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C9" t="n">
-        <v>15.956</v>
+        <v>9.827</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="G9" t="s">
-        <v>25</v>
+        <v>55</v>
       </c>
       <c r="H9" t="n">
         <v>2</v>
@@ -1146,13 +1163,13 @@
         <v>26</v>
       </c>
       <c r="K9" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="L9" t="s">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="M9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N9" t="s">
         <v>23</v>
@@ -1170,14 +1187,14 @@
         <v>1</v>
       </c>
       <c r="S9" t="n">
-        <v>-0.0056</v>
+        <v>2.0039</v>
       </c>
       <c r="T9" t="n">
         <v>2</v>
       </c>
       <c r="U9" t="s"/>
       <c r="V9" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:22">
@@ -1188,10 +1205,10 @@
         <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>4.784</v>
+        <v>15.552</v>
       </c>
       <c r="D10" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -1200,7 +1217,7 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="H10" t="n">
         <v>2</v>
@@ -1209,16 +1226,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="L10" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="M10" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N10" t="s">
         <v>23</v>
@@ -1236,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="S10" t="n">
-        <v>0.8952</v>
+        <v>0.0212</v>
       </c>
       <c r="T10" t="n">
         <v>2</v>
@@ -1248,16 +1265,16 @@
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="1" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C11" t="n">
-        <v>2.487</v>
+        <v>16.075</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
@@ -1266,7 +1283,7 @@
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H11" t="n">
         <v>2</v>
@@ -1275,16 +1292,16 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="K11" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="L11" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="M11" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N11" t="s">
         <v>23</v>
@@ -1302,55 +1319,55 @@
         <v>1</v>
       </c>
       <c r="S11" t="n">
-        <v>0.6138</v>
+        <v>-0.0056</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
       </c>
       <c r="U11" t="s"/>
       <c r="V11" t="s">
-        <v>31</v>
+        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="1" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B12" t="s">
         <v>21</v>
       </c>
       <c r="C12" t="n">
-        <v>5.976</v>
+        <v>4.925</v>
       </c>
       <c r="D12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
         <v>65</v>
       </c>
-      <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="K12" t="s">
         <v>66</v>
       </c>
-      <c r="G12" t="s">
+      <c r="L12" t="s">
         <v>67</v>
       </c>
-      <c r="H12" t="n">
-        <v>3</v>
-      </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" t="s">
-        <v>68</v>
-      </c>
-      <c r="L12" t="s">
-        <v>69</v>
-      </c>
       <c r="M12" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N12" t="s">
         <v>23</v>
@@ -1368,14 +1385,14 @@
         <v>1</v>
       </c>
       <c r="S12" t="n">
-        <v>1.3403</v>
+        <v>0.8952</v>
       </c>
       <c r="T12" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U12" t="s"/>
       <c r="V12" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:22">
@@ -1386,37 +1403,37 @@
         <v>21</v>
       </c>
       <c r="C13" t="n">
-        <v>62.252</v>
+        <v>2.235</v>
       </c>
       <c r="D13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
       </c>
       <c r="F13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" t="b">
+        <v>1</v>
+      </c>
+      <c r="J13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" t="s">
         <v>38</v>
       </c>
-      <c r="G13" t="s">
+      <c r="L13" t="s">
         <v>39</v>
       </c>
-      <c r="H13" t="n">
-        <v>3</v>
-      </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" t="s">
-        <v>42</v>
-      </c>
       <c r="M13" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N13" t="s">
         <v>23</v>
@@ -1434,12 +1451,12 @@
         <v>1</v>
       </c>
       <c r="S13" t="n">
-        <v>0.0065</v>
-      </c>
-      <c r="T13" t="s"/>
-      <c r="U13" t="n">
-        <v>3</v>
-      </c>
+        <v>0.6138</v>
+      </c>
+      <c r="T13" t="n">
+        <v>2</v>
+      </c>
+      <c r="U13" t="s"/>
       <c r="V13" t="s">
         <v>31</v>
       </c>
@@ -1452,19 +1469,19 @@
         <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>3.775</v>
+        <v>5.891</v>
       </c>
       <c r="D14" t="s">
+        <v>70</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
         <v>71</v>
       </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" t="s">
-        <v>38</v>
-      </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
@@ -1473,16 +1490,16 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="K14" t="s">
-        <v>46</v>
+        <v>73</v>
       </c>
       <c r="L14" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="M14" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="N14" t="s">
         <v>23</v>
@@ -1500,13 +1517,145 @@
         <v>1</v>
       </c>
       <c r="S14" t="n">
-        <v>0.5359</v>
+        <v>1.3403</v>
       </c>
       <c r="T14" t="n">
         <v>3</v>
       </c>
       <c r="U14" t="s"/>
       <c r="V14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="n">
+        <v>62.301</v>
+      </c>
+      <c r="D15" t="s">
+        <v>75</v>
+      </c>
+      <c r="E15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H15" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" t="b">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" t="s">
+        <v>47</v>
+      </c>
+      <c r="L15" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" t="s">
+        <v>58</v>
+      </c>
+      <c r="N15" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" t="b">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q15" t="b">
+        <v>0</v>
+      </c>
+      <c r="R15" t="b">
+        <v>1</v>
+      </c>
+      <c r="S15" t="n">
+        <v>0.0065</v>
+      </c>
+      <c r="T15" t="s"/>
+      <c r="U15" t="n">
+        <v>3</v>
+      </c>
+      <c r="V15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="n">
+        <v>3.712</v>
+      </c>
+      <c r="D16" t="s">
+        <v>76</v>
+      </c>
+      <c r="E16" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" t="s">
+        <v>44</v>
+      </c>
+      <c r="G16" t="s">
+        <v>50</v>
+      </c>
+      <c r="H16" t="n">
+        <v>3</v>
+      </c>
+      <c r="I16" t="b">
+        <v>1</v>
+      </c>
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+      <c r="K16" t="s">
+        <v>52</v>
+      </c>
+      <c r="L16" t="s">
+        <v>53</v>
+      </c>
+      <c r="M16" t="s">
+        <v>58</v>
+      </c>
+      <c r="N16" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" t="b">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q16" t="b">
+        <v>0</v>
+      </c>
+      <c r="R16" t="b">
+        <v>1</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.5359</v>
+      </c>
+      <c r="T16" t="n">
+        <v>3</v>
+      </c>
+      <c r="U16" t="s"/>
+      <c r="V16" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated Result table after test color update
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="76">
   <si>
     <t>Bound_cond</t>
   </si>
@@ -113,75 +113,72 @@
     <t>Green</t>
   </si>
   <si>
+    <t>[0.17381931436989675, 0.015704630897802694, 0.0050889346986909955, 0.0008049994197372305, 0.00020964279836201426]</t>
+  </si>
+  <si>
+    <t>squareWithDelaunayTriangles</t>
+  </si>
+  <si>
+    <t>[u'squareWithTriangles_1', u'squareWithTriangles_2', u'squareWithTriangles_3', u'squareWithTriangles_4', u'squareWithTriangles_5']</t>
+  </si>
+  <si>
+    <t>[6.32455532033676, 14.966629547095765, 30.561413579872255, 80.13738203859668, 160.8477541030648]</t>
+  </si>
+  <si>
+    <t>Unstructured_triangles</t>
+  </si>
+  <si>
     <t>Neumann</t>
   </si>
   <si>
     <t>[0.7503307283176518, 0.2539544973957279, 0.10870368061041591, 0.055777341080608625, 0.028297242335636467, 0.014264092354052018]</t>
   </si>
   <si>
-    <t>Orange (ILU)</t>
-  </si>
-  <si>
-    <t>[0.17381931436989675, 0.015704630897802694, 0.0050889346986909955, 0.0008049994197372305, 0.00020964279836201426]</t>
-  </si>
-  <si>
-    <t>squareWithDelaunayTriangles</t>
-  </si>
-  <si>
-    <t>[u'squareWithTriangles_1', u'squareWithTriangles_2', u'squareWithTriangles_3', u'squareWithTriangles_4', u'squareWithTriangles_5']</t>
-  </si>
-  <si>
-    <t>[6.32455532033676, 14.966629547095765, 30.561413579872255, 80.13738203859668, 160.8477541030648]</t>
-  </si>
-  <si>
-    <t>Unstructured_triangles</t>
+    <t>Orange (not order 2)</t>
   </si>
   <si>
     <t>[0.6631505332206331, 0.39408058878012564, 0.21896100196675858, 0.09151553643693577, 0.04861943552271186]</t>
   </si>
   <si>
+    <t>[0.033558391102700875, 0.008265416966230732, 0.0020587067645389525, 0.0009143535530498623]</t>
+  </si>
+  <si>
+    <t>Tetrahedron</t>
+  </si>
+  <si>
+    <t>cubeWithRegularTetrahedra</t>
+  </si>
+  <si>
+    <t>[5, 10, 20, 30]</t>
+  </si>
+  <si>
+    <t>[27.386127875258307, 77.45966692414835, 219.08902300206654, 402.4922359499621]</t>
+  </si>
+  <si>
+    <t>Regular_Tetrahedra</t>
+  </si>
+  <si>
+    <t>[0.15982423149490765, 0.19209081782655904, 0.02588837716517572, 0.10154356764807221, 0.04012117422231292]</t>
+  </si>
+  <si>
+    <t>cubeWithDelaunayTetrahedra</t>
+  </si>
+  <si>
+    <t>[u'meshCubeTetrahedra_0', u'meshCubeTetrahedra_1', u'meshCubeTetrahedra_2', u'meshCubeTetrahedra_3', u'meshCubeTetrahedra_4']</t>
+  </si>
+  <si>
+    <t>[16.431676725154983, 45.617978911828175, 63.85138996137828, 87.34414691323053, 129.74590552306458]</t>
+  </si>
+  <si>
+    <t>Unstructured_Tetrahedra</t>
+  </si>
+  <si>
+    <t>[0.0335583911027002, 0.0020587067645353673, 0.0003290517629436336, 8.22507622070037e-05, 2.0561929520719267e-05, 5.140434811781161e-06]</t>
+  </si>
+  <si>
     <t>Squares</t>
   </si>
   <si>
-    <t>Red</t>
-  </si>
-  <si>
-    <t>[0.033558391102700875, 0.008265416966230732, 0.0020587067645389525, 0.0009143535530498623]</t>
-  </si>
-  <si>
-    <t>Tetrahedron</t>
-  </si>
-  <si>
-    <t>cubeWithRegularTetrahedra</t>
-  </si>
-  <si>
-    <t>[5, 10, 20, 30]</t>
-  </si>
-  <si>
-    <t>[27.386127875258307, 77.45966692414835, 219.08902300206654, 402.4922359499621]</t>
-  </si>
-  <si>
-    <t>Regular_Tetrahedra</t>
-  </si>
-  <si>
-    <t>[0.15982423149490765, 0.19209081782655904, 0.02588837716517572, 0.10154356764807221, 0.04012117422231292]</t>
-  </si>
-  <si>
-    <t>cubeWithDelaunayTetrahedra</t>
-  </si>
-  <si>
-    <t>[u'meshCubeTetrahedra_0', u'meshCubeTetrahedra_1', u'meshCubeTetrahedra_2', u'meshCubeTetrahedra_3', u'meshCubeTetrahedra_4']</t>
-  </si>
-  <si>
-    <t>[16.431676725154983, 45.617978911828175, 63.85138996137828, 87.34414691323053, 129.74590552306458]</t>
-  </si>
-  <si>
-    <t>Unstructured_Tetrahedra</t>
-  </si>
-  <si>
-    <t>[0.0335583911027002, 0.0020587067645353673, 0.0003290517629436336, 8.22507622070037e-05, 2.0561929520719267e-05, 5.140434811781161e-06]</t>
-  </si>
-  <si>
     <t>squareWithSquares</t>
   </si>
   <si>
@@ -194,10 +191,32 @@
     <t>FV</t>
   </si>
   <si>
+    <t>[0.0669509874804482, 0.06815847506446479, 0.06471965034394461, 0.06325778881561246, 0.06255657471840613, 0.06218973390644179]</t>
+  </si>
+  <si>
+    <t>[0.1450449320264222, 0.043301182264762685, 0.017799215386138302, 0.012676403707012044, 0.004513492486842332]</t>
+  </si>
+  <si>
+    <t>squareWithEquilateralTriangles</t>
+  </si>
+  <si>
+    <t>[u'squareWithEquilateralTriangles5', u'squareWithEquilateralTriangles20', u'squareWithEquilateralTriangles50', u'squareWithEquilateralTriangles100', u'squareWithEquilateralTriangles200']</t>
+  </si>
+  <si>
+    <t>[6.32455532033676, 26.07680962081059, 65.57438524302002, 131.14877048603998, 263.058928759318]</t>
+  </si>
+  <si>
+    <t>Structured_triangles</t>
+  </si>
+  <si>
+    <t>Orange 
+ (BC don't fit the domain)</t>
+  </si>
+  <si>
+    <t>[0.04972168575894865, 0.04358040486275293, 0.02190713533101905, 0.011510133471144974, 0.007903217495358324]</t>
+  </si>
+  <si>
     <t>[0.0335583911027001, 0.002058706764536365, 0.000329051762941964, 8.225076224220633e-05, 2.0561929538928084e-05, 5.140434875730902e-06]</t>
-  </si>
-  <si>
-    <t>[0.0669509874804482, 0.06815847506446479, 0.06471965034394461, 0.06325778881561246, 0.06255657471840613, 0.06218973390644179]</t>
   </si>
   <si>
     <t>[0.20788601050300354, 0.21324870454359207, 0.21369860273963248, 0.21376283055789733, 0.21377888577341903, 0.21378289946864626]</t>
@@ -205,28 +224,6 @@
   <si>
     <t>Orange 
  (suspicious order 0 convergence)</t>
-  </si>
-  <si>
-    <t>[0.1450449320264222, 0.043301182264762685, 0.017799215386138302, 0.012676403707012044, 0.004513492486842332]</t>
-  </si>
-  <si>
-    <t>squareWithEquilateralTriangles</t>
-  </si>
-  <si>
-    <t>[u'squareWithEquilateralTriangles5', u'squareWithEquilateralTriangles20', u'squareWithEquilateralTriangles50', u'squareWithEquilateralTriangles100', u'squareWithEquilateralTriangles200']</t>
-  </si>
-  <si>
-    <t>[6.32455532033676, 26.07680962081059, 65.57438524302002, 131.14877048603998, 263.058928759318]</t>
-  </si>
-  <si>
-    <t>Structured_triangles</t>
-  </si>
-  <si>
-    <t>Orange 
- (BC don't fit the domain)</t>
-  </si>
-  <si>
-    <t>[0.04972168575894865, 0.04358040486275293, 0.02190713533101905, 0.011510133471144974, 0.007903217495358324]</t>
   </si>
   <si>
     <t>[0.03355839110270013, 0.00826541696622572, 0.0020587067645243596, 0.0009143535530931283]</t>
@@ -677,7 +674,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="n">
-        <v>103.069</v>
+        <v>103.144</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -737,16 +734,16 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" s="1" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6.093</v>
+      </c>
+      <c r="D3" t="s">
         <v>32</v>
-      </c>
-      <c r="C3" t="n">
-        <v>26.158</v>
-      </c>
-      <c r="D3" t="s">
-        <v>33</v>
       </c>
       <c r="E3" t="s">
         <v>23</v>
@@ -755,7 +752,7 @@
         <v>24</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H3" t="n">
         <v>2</v>
@@ -764,13 +761,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="M3" t="s">
         <v>29</v>
@@ -791,28 +788,28 @@
         <v>1</v>
       </c>
       <c r="S3" t="n">
-        <v>0.9103</v>
+        <v>2.0156</v>
       </c>
       <c r="T3" t="n">
         <v>2</v>
       </c>
       <c r="U3" t="s"/>
       <c r="V3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:22">
       <c r="A4" s="1" t="n">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C4" t="n">
-        <v>7.609</v>
+        <v>26.25</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
         <v>23</v>
@@ -821,7 +818,7 @@
         <v>24</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H4" t="n">
         <v>2</v>
@@ -830,13 +827,13 @@
         <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="K4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="M4" t="s">
         <v>29</v>
@@ -857,14 +854,14 @@
         <v>1</v>
       </c>
       <c r="S4" t="n">
-        <v>2.0156</v>
+        <v>0.9103</v>
       </c>
       <c r="T4" t="n">
         <v>2</v>
       </c>
       <c r="U4" t="s"/>
       <c r="V4" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:22">
@@ -872,10 +869,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C5" t="n">
-        <v>3.102</v>
+        <v>3.179</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -884,25 +881,25 @@
         <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" t="s">
+        <v>35</v>
+      </c>
+      <c r="L5" t="s">
         <v>36</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" t="s">
-        <v>39</v>
       </c>
       <c r="M5" t="s">
         <v>29</v>
@@ -930,7 +927,7 @@
       </c>
       <c r="U5" t="s"/>
       <c r="V5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:22">
@@ -941,19 +938,19 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>208.494</v>
+        <v>208.857</v>
       </c>
       <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
         <v>43</v>
-      </c>
-      <c r="E6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
       </c>
       <c r="H6" t="n">
         <v>3</v>
@@ -962,13 +959,13 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
+        <v>44</v>
+      </c>
+      <c r="K6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" t="s">
         <v>46</v>
-      </c>
-      <c r="K6" t="s">
-        <v>47</v>
-      </c>
-      <c r="L6" t="s">
-        <v>48</v>
       </c>
       <c r="M6" t="s">
         <v>29</v>
@@ -996,7 +993,7 @@
       </c>
       <c r="U6" t="s"/>
       <c r="V6" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:22">
@@ -1007,19 +1004,19 @@
         <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>12.001</v>
+        <v>11.857</v>
       </c>
       <c r="D7" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H7" t="n">
         <v>3</v>
@@ -1028,13 +1025,13 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
+        <v>49</v>
+      </c>
+      <c r="K7" t="s">
+        <v>50</v>
+      </c>
+      <c r="L7" t="s">
         <v>51</v>
-      </c>
-      <c r="K7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L7" t="s">
-        <v>53</v>
       </c>
       <c r="M7" t="s">
         <v>29</v>
@@ -1062,7 +1059,7 @@
       </c>
       <c r="U7" t="s"/>
       <c r="V7" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:22">
@@ -1073,19 +1070,19 @@
         <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>9.776999999999999</v>
+        <v>9.807</v>
       </c>
       <c r="D8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" t="s">
         <v>54</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" t="s">
-        <v>55</v>
       </c>
       <c r="H8" t="n">
         <v>2</v>
@@ -1097,13 +1094,13 @@
         <v>26</v>
       </c>
       <c r="K8" t="s">
+        <v>55</v>
+      </c>
+      <c r="L8" t="s">
         <v>56</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>57</v>
-      </c>
-      <c r="M8" t="s">
-        <v>58</v>
       </c>
       <c r="N8" t="s">
         <v>23</v>
@@ -1133,25 +1130,25 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="n">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C9" t="n">
-        <v>9.827</v>
+        <v>15.593</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>25</v>
       </c>
       <c r="H9" t="n">
         <v>2</v>
@@ -1163,13 +1160,13 @@
         <v>26</v>
       </c>
       <c r="K9" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="L9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" t="s">
         <v>57</v>
-      </c>
-      <c r="M9" t="s">
-        <v>58</v>
       </c>
       <c r="N9" t="s">
         <v>23</v>
@@ -1187,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="S9" t="n">
-        <v>2.0039</v>
+        <v>0.0212</v>
       </c>
       <c r="T9" t="n">
         <v>2</v>
@@ -1199,16 +1196,16 @@
     </row>
     <row r="10" spans="1:22">
       <c r="A10" s="1" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" t="s">
         <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>15.552</v>
+        <v>4.73</v>
       </c>
       <c r="D10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -1217,7 +1214,7 @@
         <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="H10" t="n">
         <v>2</v>
@@ -1226,16 +1223,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="L10" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="M10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N10" t="s">
         <v>23</v>
@@ -1253,28 +1250,28 @@
         <v>1</v>
       </c>
       <c r="S10" t="n">
-        <v>0.0212</v>
+        <v>0.8952</v>
       </c>
       <c r="T10" t="n">
         <v>2</v>
       </c>
       <c r="U10" t="s"/>
       <c r="V10" t="s">
-        <v>31</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:22">
       <c r="A11" s="1" t="n">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C11" t="n">
-        <v>16.075</v>
+        <v>2.264</v>
       </c>
       <c r="D11" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
@@ -1283,7 +1280,7 @@
         <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="H11" t="n">
         <v>2</v>
@@ -1292,16 +1289,16 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="L11" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="M11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N11" t="s">
         <v>23</v>
@@ -1319,37 +1316,37 @@
         <v>1</v>
       </c>
       <c r="S11" t="n">
-        <v>-0.0056</v>
+        <v>0.6138</v>
       </c>
       <c r="T11" t="n">
         <v>2</v>
       </c>
       <c r="U11" t="s"/>
       <c r="V11" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:22">
       <c r="A12" s="1" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C12" t="n">
-        <v>4.925</v>
+        <v>9.804</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
         <v>23</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="G12" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H12" t="n">
         <v>2</v>
@@ -1358,16 +1355,16 @@
         <v>1</v>
       </c>
       <c r="J12" t="s">
-        <v>65</v>
+        <v>26</v>
       </c>
       <c r="K12" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="M12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N12" t="s">
         <v>23</v>
@@ -1385,28 +1382,28 @@
         <v>1</v>
       </c>
       <c r="S12" t="n">
-        <v>0.8952</v>
+        <v>2.0039</v>
       </c>
       <c r="T12" t="n">
         <v>2</v>
       </c>
       <c r="U12" t="s"/>
       <c r="V12" t="s">
-        <v>68</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:22">
       <c r="A13" s="1" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>2.235</v>
+        <v>15.944</v>
       </c>
       <c r="D13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1415,7 +1412,7 @@
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="H13" t="n">
         <v>2</v>
@@ -1424,16 +1421,16 @@
         <v>1</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="K13" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="L13" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="M13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N13" t="s">
         <v>23</v>
@@ -1451,14 +1448,14 @@
         <v>1</v>
       </c>
       <c r="S13" t="n">
-        <v>0.6138</v>
+        <v>-0.0056</v>
       </c>
       <c r="T13" t="n">
         <v>2</v>
       </c>
       <c r="U13" t="s"/>
       <c r="V13" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:22">
@@ -1469,19 +1466,19 @@
         <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>5.891</v>
+        <v>5.738</v>
       </c>
       <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>23</v>
+      </c>
+      <c r="F14" t="s">
         <v>70</v>
       </c>
-      <c r="E14" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>71</v>
-      </c>
-      <c r="G14" t="s">
-        <v>72</v>
       </c>
       <c r="H14" t="n">
         <v>3</v>
@@ -1490,16 +1487,16 @@
         <v>1</v>
       </c>
       <c r="J14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L14" t="s">
         <v>73</v>
       </c>
-      <c r="L14" t="s">
-        <v>74</v>
-      </c>
       <c r="M14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N14" t="s">
         <v>23</v>
@@ -1524,7 +1521,7 @@
       </c>
       <c r="U14" t="s"/>
       <c r="V14" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:22">
@@ -1535,19 +1532,19 @@
         <v>21</v>
       </c>
       <c r="C15" t="n">
-        <v>62.301</v>
+        <v>61.84</v>
       </c>
       <c r="D15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E15" t="s">
         <v>23</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H15" t="n">
         <v>3</v>
@@ -1556,16 +1553,16 @@
         <v>1</v>
       </c>
       <c r="J15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" t="s">
+        <v>45</v>
+      </c>
+      <c r="L15" t="s">
         <v>46</v>
       </c>
-      <c r="K15" t="s">
-        <v>47</v>
-      </c>
-      <c r="L15" t="s">
-        <v>48</v>
-      </c>
       <c r="M15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N15" t="s">
         <v>23</v>
@@ -1590,7 +1587,7 @@
         <v>3</v>
       </c>
       <c r="V15" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -1601,19 +1598,19 @@
         <v>21</v>
       </c>
       <c r="C16" t="n">
-        <v>3.712</v>
+        <v>3.572</v>
       </c>
       <c r="D16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E16" t="s">
         <v>23</v>
       </c>
       <c r="F16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H16" t="n">
         <v>3</v>
@@ -1622,16 +1619,16 @@
         <v>1</v>
       </c>
       <c r="J16" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" t="s">
+        <v>50</v>
+      </c>
+      <c r="L16" t="s">
         <v>51</v>
       </c>
-      <c r="K16" t="s">
-        <v>52</v>
-      </c>
-      <c r="L16" t="s">
-        <v>53</v>
-      </c>
       <c r="M16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N16" t="s">
         <v>23</v>
@@ -1656,7 +1653,7 @@
       </c>
       <c r="U16" t="s"/>
       <c r="V16" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated convergence test table
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
@@ -674,7 +674,7 @@
         <v>21</v>
       </c>
       <c r="C2" t="n">
-        <v>103.144</v>
+        <v>104.198</v>
       </c>
       <c r="D2" t="s">
         <v>22</v>
@@ -740,7 +740,7 @@
         <v>21</v>
       </c>
       <c r="C3" t="n">
-        <v>6.093</v>
+        <v>6.22</v>
       </c>
       <c r="D3" t="s">
         <v>32</v>
@@ -806,7 +806,7 @@
         <v>37</v>
       </c>
       <c r="C4" t="n">
-        <v>26.25</v>
+        <v>26.242</v>
       </c>
       <c r="D4" t="s">
         <v>38</v>
@@ -872,7 +872,7 @@
         <v>37</v>
       </c>
       <c r="C5" t="n">
-        <v>3.179</v>
+        <v>3.072</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -938,7 +938,7 @@
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>208.857</v>
+        <v>210.918</v>
       </c>
       <c r="D6" t="s">
         <v>41</v>
@@ -1004,7 +1004,7 @@
         <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>11.857</v>
+        <v>11.879</v>
       </c>
       <c r="D7" t="s">
         <v>47</v>
@@ -1070,7 +1070,7 @@
         <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>9.807</v>
+        <v>9.888999999999999</v>
       </c>
       <c r="D8" t="s">
         <v>52</v>
@@ -1136,7 +1136,7 @@
         <v>21</v>
       </c>
       <c r="C9" t="n">
-        <v>15.593</v>
+        <v>15.589</v>
       </c>
       <c r="D9" t="s">
         <v>58</v>
@@ -1202,7 +1202,7 @@
         <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>4.73</v>
+        <v>4.776</v>
       </c>
       <c r="D10" t="s">
         <v>59</v>
@@ -1268,7 +1268,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="n">
-        <v>2.264</v>
+        <v>2.244</v>
       </c>
       <c r="D11" t="s">
         <v>65</v>
@@ -1334,7 +1334,7 @@
         <v>37</v>
       </c>
       <c r="C12" t="n">
-        <v>9.804</v>
+        <v>9.765000000000001</v>
       </c>
       <c r="D12" t="s">
         <v>66</v>
@@ -1400,7 +1400,7 @@
         <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>15.944</v>
+        <v>15.772</v>
       </c>
       <c r="D13" t="s">
         <v>67</v>
@@ -1466,7 +1466,7 @@
         <v>21</v>
       </c>
       <c r="C14" t="n">
-        <v>5.738</v>
+        <v>6.143</v>
       </c>
       <c r="D14" t="s">
         <v>69</v>
@@ -1532,7 +1532,7 @@
         <v>21</v>
       </c>
       <c r="C15" t="n">
-        <v>61.84</v>
+        <v>62.615</v>
       </c>
       <c r="D15" t="s">
         <v>74</v>
@@ -1587,7 +1587,7 @@
         <v>3</v>
       </c>
       <c r="V15" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:22">
@@ -1598,7 +1598,7 @@
         <v>21</v>
       </c>
       <c r="C16" t="n">
-        <v>3.572</v>
+        <v>3.962</v>
       </c>
       <c r="D16" t="s">
         <v>75</v>
@@ -1653,7 +1653,7 @@
       </c>
       <c r="U16" t="s"/>
       <c r="V16" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected display errors in convergence table
</commit_message>
<xml_diff>
--- a/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
+++ b/examples/Python/Convergence/StationaryDiffusion/synthesis/convergence_synthesis_StationaryDiffusion_all.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="71">
   <si>
     <t>Bound_cond</t>
   </si>
@@ -149,6 +149,33 @@
     <t>Orange (not order 2)</t>
   </si>
   <si>
+    <t>[0.0669509874804482, 0.0681584750644647, 0.0647196503439448, 0.06325778881561307, 0.06255657471840799, 0.062189733906443063]</t>
+  </si>
+  <si>
+    <t>FV</t>
+  </si>
+  <si>
+    <t>[0.04972168575894878, 0.04358040486275293, 0.021907135331019106, 0.011510133471144197, 0.007903217495355106]</t>
+  </si>
+  <si>
+    <t>[0.046876674938071156, 0.005343400720956583, 0.0013517237061705155, 0.0004892479591165943, 0.0001228308963559409]</t>
+  </si>
+  <si>
+    <t>Hexagons</t>
+  </si>
+  <si>
+    <t>squareWithHexagons</t>
+  </si>
+  <si>
+    <t>[u'squareWithHexagons_1', u'squareWithHexagons_2', u'squareWithHexagons_3', u'squareWithHexagons_4', u'squareWithHexagons_5']</t>
+  </si>
+  <si>
+    <t>[5.000000000000001, 15.96871942267131, 31.937438845342623, 53.38539126015656, 107.23805294763609]</t>
+  </si>
+  <si>
+    <t>Structured_hexagons</t>
+  </si>
+  <si>
     <t>[0.021631644879469406, 0.0013678634059067934, 0.00021897475093210793, 5.478038078209184e-05, 1.370105945151739e-05]</t>
   </si>
   <si>
@@ -164,13 +191,6 @@
     <t>Equilateral_triangles</t>
   </si>
   <si>
-    <t>FV</t>
-  </si>
-  <si>
-    <t>Orange 
- (BC don't fit the domain)</t>
-  </si>
-  <si>
     <t>[0.03355839110269998, 0.002058706764535256, 0.0003290517629437446, 8.225076220744793e-05, 2.0561929520497192e-05, 5.1404348144457395e-06]</t>
   </si>
   <si>
@@ -184,30 +204,6 @@
   </si>
   <si>
     <t>RegularSquares</t>
-  </si>
-  <si>
-    <t>[0.0669509874804482, 0.0681584750644647, 0.0647196503439448, 0.06325778881561307, 0.06255657471840799, 0.062189733906443063]</t>
-  </si>
-  <si>
-    <t>[0.046876674938071156, 0.005343400720956583, 0.0013517237061705155, 0.0004892479591165943, 0.0001228308963559409]</t>
-  </si>
-  <si>
-    <t>Hexagons</t>
-  </si>
-  <si>
-    <t>squareWithHexagons</t>
-  </si>
-  <si>
-    <t>[u'squareWithHexagons_1', u'squareWithHexagons_2', u'squareWithHexagons_3', u'squareWithHexagons_4', u'squareWithHexagons_5']</t>
-  </si>
-  <si>
-    <t>[5.000000000000001, 15.96871942267131, 31.937438845342623, 53.38539126015656, 107.23805294763609]</t>
-  </si>
-  <si>
-    <t>Unstructured_hexagons</t>
-  </si>
-  <si>
-    <t>[0.04972168575894878, 0.04358040486275293, 0.021907135331019106, 0.011510133471144197, 0.007903217495355106]</t>
   </si>
   <si>
     <t>[0.08220526266791427, 0.08443932671400403, 0.08219454187484591, 0.0811274246865842]</t>
@@ -853,13 +849,13 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" s="1" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>5.137</v>
+        <v>17.547</v>
       </c>
       <c r="D5" t="s">
         <v>44</v>
@@ -871,25 +867,25 @@
         <v>24</v>
       </c>
       <c r="G5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" t="b">
+        <v>1</v>
+      </c>
+      <c r="J5" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
         <v>45</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K5" t="s">
-        <v>47</v>
-      </c>
-      <c r="L5" t="s">
-        <v>48</v>
-      </c>
-      <c r="M5" t="s">
-        <v>49</v>
       </c>
       <c r="N5" t="s">
         <v>23</v>
@@ -907,37 +903,37 @@
         <v>1</v>
       </c>
       <c r="S5" t="n">
-        <v>1.9766</v>
+        <v>0.0212</v>
       </c>
       <c r="T5" t="n">
         <v>2</v>
       </c>
       <c r="U5" t="s"/>
       <c r="V5" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:22">
       <c r="A6" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="C6" t="n">
-        <v>10.755</v>
+        <v>2.386</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>
       <c r="F6" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="H6" t="n">
         <v>2</v>
@@ -946,16 +942,16 @@
         <v>1</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="K6" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
       <c r="L6" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="M6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N6" t="s">
         <v>23</v>
@@ -973,7 +969,7 @@
         <v>1</v>
       </c>
       <c r="S6" t="n">
-        <v>2.0039</v>
+        <v>0.6138</v>
       </c>
       <c r="T6" t="n">
         <v>2</v>
@@ -985,25 +981,25 @@
     </row>
     <row r="7" spans="1:22">
       <c r="A7" s="1" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
       </c>
       <c r="C7" t="n">
-        <v>17.547</v>
+        <v>2.38</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
         <v>23</v>
       </c>
       <c r="F7" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
-        <v>25</v>
+        <v>49</v>
       </c>
       <c r="H7" t="n">
         <v>2</v>
@@ -1012,16 +1008,16 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="L7" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="M7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N7" t="s">
         <v>23</v>
@@ -1039,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="S7" t="n">
-        <v>0.0212</v>
+        <v>1.9416</v>
       </c>
       <c r="T7" t="n">
         <v>2</v>
@@ -1051,43 +1047,43 @@
     </row>
     <row r="8" spans="1:22">
       <c r="A8" s="1" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8" t="n">
-        <v>2.261</v>
+        <v>5.698</v>
       </c>
       <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>54</v>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" t="b">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>55</v>
+      </c>
+      <c r="K8" t="s">
+        <v>56</v>
+      </c>
+      <c r="L8" t="s">
         <v>57</v>
       </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" t="s">
-        <v>59</v>
-      </c>
-      <c r="H8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="s">
-        <v>60</v>
-      </c>
-      <c r="K8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" t="s">
-        <v>62</v>
-      </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N8" t="s">
         <v>23</v>
@@ -1105,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="S8" t="n">
-        <v>1.9416</v>
+        <v>1.9766</v>
       </c>
       <c r="T8" t="n">
         <v>2</v>
@@ -1117,25 +1113,25 @@
     </row>
     <row r="9" spans="1:22">
       <c r="A9" s="1" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9" t="n">
-        <v>2.386</v>
+        <v>10.755</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E9" t="s">
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="H9" t="n">
         <v>2</v>
@@ -1144,16 +1140,16 @@
         <v>1</v>
       </c>
       <c r="J9" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="M9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N9" t="s">
         <v>23</v>
@@ -1171,7 +1167,7 @@
         <v>1</v>
       </c>
       <c r="S9" t="n">
-        <v>0.6138</v>
+        <v>2.0039</v>
       </c>
       <c r="T9" t="n">
         <v>2</v>
@@ -1192,7 +1188,7 @@
         <v>76.646</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
         <v>23</v>
@@ -1201,7 +1197,7 @@
         <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H10" t="n">
         <v>3</v>
@@ -1210,16 +1206,16 @@
         <v>1</v>
       </c>
       <c r="J10" t="s">
+        <v>65</v>
+      </c>
+      <c r="K10" t="s">
         <v>66</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>67</v>
       </c>
-      <c r="L10" t="s">
-        <v>68</v>
-      </c>
       <c r="M10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N10" t="s">
         <v>23</v>
@@ -1258,7 +1254,7 @@
         <v>19.588</v>
       </c>
       <c r="D11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
@@ -1276,16 +1272,16 @@
         <v>1</v>
       </c>
       <c r="J11" t="s">
+        <v>69</v>
+      </c>
+      <c r="K11" t="s">
         <v>70</v>
-      </c>
-      <c r="K11" t="s">
-        <v>71</v>
       </c>
       <c r="L11" t="s">
         <v>42</v>
       </c>
       <c r="M11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="N11" t="s">
         <v>23</v>

</xml_diff>